<commit_message>
create metadata for deployment, project
</commit_message>
<xml_diff>
--- a/input/attributes_cameras.xlsx
+++ b/input/attributes_cameras.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\wildlife-cameras\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E57A1DB5-77F1-48C4-B6F9-F6422E745DBB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFC6C24-DDA7-46A8-A971-4ADE4E789842}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21495" windowHeight="11640" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21495" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attributes_cameras" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">camera_sn_dates!$A$1:$E$1069</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'serial-numbers'!$A$1:$K$187</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -1382,9 +1382,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1938,15 +1938,15 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2435,11 +2435,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="J1" sqref="J1:K1048576"/>
@@ -7488,16 +7488,16 @@
       <c r="AU55" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AV55"/>
+  <autoFilter ref="A1:AV55" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M187"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:K187"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -12406,7 +12406,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K187"/>
+  <autoFilter ref="A1:K187" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <sortState ref="A2:M187">
     <sortCondition ref="F2:F187"/>
     <sortCondition ref="E2:E187"/>
@@ -12475,7 +12475,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E225"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -16188,7 +16188,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1069"/>
+  <autoFilter ref="A1:E1069" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <sortState ref="A2:E225">
     <sortCondition ref="A2:A225"/>
     <sortCondition ref="B2:B225"/>

</xml_diff>